<commit_message>
Working list of dictionaries.
</commit_message>
<xml_diff>
--- a/test_sheet.xlsx
+++ b/test_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\state_req\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BCF8C2-2C26-4AC6-AE3E-037461E59B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FB264C-7AFD-4F6D-9D5B-EF295C73C220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14445" yWindow="90" windowWidth="14265" windowHeight="15420" xr2:uid="{11619111-E7E6-4665-8C0A-DE0CFA2CAEA8}"/>
+    <workbookView xWindow="16320" yWindow="90" windowWidth="12390" windowHeight="15420" xr2:uid="{11619111-E7E6-4665-8C0A-DE0CFA2CAEA8}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>Apple</t>
   </si>
@@ -117,6 +117,39 @@
   </si>
   <si>
     <t>schedule 9</t>
+  </si>
+  <si>
+    <t>https://www.chadjemmett.com1</t>
+  </si>
+  <si>
+    <t>https://www.chadjemmett.com2</t>
+  </si>
+  <si>
+    <t>https://www.chadjemmett.com3</t>
+  </si>
+  <si>
+    <t>https://www.chadjemmett.com4</t>
+  </si>
+  <si>
+    <t>https://www.chadjemmett.com5</t>
+  </si>
+  <si>
+    <t>www.google.com</t>
+  </si>
+  <si>
+    <t>www.boinggoin.com</t>
+  </si>
+  <si>
+    <t>www.facebooko.com</t>
+  </si>
+  <si>
+    <t>www.metafileter.com</t>
+  </si>
+  <si>
+    <t>www.bobo.com</t>
+  </si>
+  <si>
+    <t>www.twitch.com</t>
   </si>
 </sst>
 </file>
@@ -512,7 +545,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +619,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -594,7 +627,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -602,7 +635,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -610,7 +643,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -618,7 +651,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -626,7 +659,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -655,7 +688,7 @@
         <v>21</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,7 +696,7 @@
         <v>22</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -671,7 +704,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -679,7 +712,7 @@
         <v>24</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -687,7 +720,7 @@
         <v>25</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -695,7 +728,7 @@
         <v>26</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>